<commit_message>
labels from ros report
</commit_message>
<xml_diff>
--- a/report/ros.xlsx
+++ b/report/ros.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t>DATA</t>
   </si>
@@ -55,6 +55,48 @@
     <t>RESPONSAVEL</t>
   </si>
   <si>
+    <t>26-01-2023 14:10</t>
+  </si>
+  <si>
+    <t>jan</t>
+  </si>
+  <si>
+    <t>2023</t>
+  </si>
+  <si>
+    <t>Anônimo</t>
+  </si>
+  <si>
+    <t>Portaria</t>
+  </si>
+  <si>
+    <t>Planta Industrial</t>
+  </si>
+  <si>
+    <t>Meio Ambiente</t>
+  </si>
+  <si>
+    <t>Falta de limpeza e organização</t>
+  </si>
+  <si>
+    <t>rerrerere</t>
+  </si>
+  <si>
+    <t>adadada</t>
+  </si>
+  <si>
+    <t>Tratado</t>
+  </si>
+  <si>
+    <t>Resolvido</t>
+  </si>
+  <si>
+    <t>ADM</t>
+  </si>
+  <si>
+    <t>Jorge Leandro Nunes de Oliveira</t>
+  </si>
+  <si>
     <t>01-11-2022 16:11</t>
   </si>
   <si>
@@ -64,19 +106,7 @@
     <t>2022</t>
   </si>
   <si>
-    <t>Anônimo</t>
-  </si>
-  <si>
-    <t>zoneData.find(zone =&gt; zone.id === ros.zone_id).name</t>
-  </si>
-  <si>
-    <t>localData.find(local =&gt; local.id === ros.local_id).name</t>
-  </si>
-  <si>
-    <t>natureData.find(nature =&gt; nature.id === ros.nature_id).name</t>
-  </si>
-  <si>
-    <t>reasonData.find(reason =&gt; reason.id === ros.reason_id).name</t>
+    <t>João Fernando dos Santos</t>
   </si>
   <si>
     <t>isdaisdiahs</t>
@@ -91,10 +121,7 @@
     <t>não resolvido</t>
   </si>
   <si>
-    <t>responsibleAreaData.find(responsible =&gt; responsible.id === ros.responsible_area_id).name</t>
-  </si>
-  <si>
-    <t>usersData.find(responsible =&gt; responsible.id === ros.responsible_id).name</t>
+    <t/>
   </si>
   <si>
     <t>01-11-2022 16:03</t>
@@ -112,6 +139,9 @@
     <t>ago</t>
   </si>
   <si>
+    <t>Barragem de rejeito</t>
+  </si>
+  <si>
     <t>teste</t>
   </si>
   <si>
@@ -139,18 +169,18 @@
     <t>out</t>
   </si>
   <si>
+    <t>Segurança do Trabalho</t>
+  </si>
+  <si>
+    <t>Falta do uso do EPI</t>
+  </si>
+  <si>
     <t>tetsteyewttae</t>
   </si>
   <si>
     <t>asjdijasidjaisj</t>
   </si>
   <si>
-    <t>Tratado</t>
-  </si>
-  <si>
-    <t>Resolvido</t>
-  </si>
-  <si>
     <t>04-10-2022 08:34</t>
   </si>
   <si>
@@ -169,6 +199,9 @@
     <t>Alterar responsvel</t>
   </si>
   <si>
+    <t>TI</t>
+  </si>
+  <si>
     <t>30-09-2022 16:15</t>
   </si>
   <si>
@@ -185,6 +218,9 @@
   </si>
   <si>
     <t>Não Resolvido</t>
+  </si>
+  <si>
+    <t>Admin</t>
   </si>
 </sst>
 </file>
@@ -230,7 +266,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N15"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
@@ -329,13 +365,13 @@
         <v>28</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>18</v>
@@ -350,33 +386,33 @@
         <v>21</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="N3" s="0" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="0" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>17</v>
@@ -394,33 +430,33 @@
         <v>21</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="M4" s="0" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="N4" s="0" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="0" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>17</v>
@@ -429,7 +465,7 @@
         <v>18</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="G5" s="0" t="s">
         <v>20</v>
@@ -438,33 +474,33 @@
         <v>21</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="L5" s="0" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="M5" s="0" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="N5" s="0" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="0" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>17</v>
@@ -473,7 +509,7 @@
         <v>18</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="G6" s="0" t="s">
         <v>20</v>
@@ -482,33 +518,33 @@
         <v>21</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="L6" s="0" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="M6" s="0" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="N6" s="0" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="0" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>17</v>
@@ -517,7 +553,7 @@
         <v>18</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="G7" s="0" t="s">
         <v>20</v>
@@ -526,33 +562,33 @@
         <v>21</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="L7" s="0" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="M7" s="0" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="N7" s="0" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="0" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>17</v>
@@ -561,7 +597,7 @@
         <v>18</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="G8" s="0" t="s">
         <v>20</v>
@@ -570,33 +606,33 @@
         <v>21</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="K8" s="0" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="L8" s="0" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="M8" s="0" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="N8" s="0" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="0" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>17</v>
@@ -605,7 +641,7 @@
         <v>18</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="G9" s="0" t="s">
         <v>20</v>
@@ -614,33 +650,33 @@
         <v>21</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="K9" s="0" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="L9" s="0" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="M9" s="0" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="N9" s="0" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="0" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>17</v>
@@ -658,33 +694,33 @@
         <v>21</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="L10" s="0" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="M10" s="0" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="N10" s="0" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="0" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>17</v>
@@ -702,33 +738,33 @@
         <v>21</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="K11" s="0" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="L11" s="0" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="M11" s="0" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="N11" s="0" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:14">
       <c r="A12" s="0" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>17</v>
@@ -746,36 +782,36 @@
         <v>21</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="K12" s="0" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="L12" s="0" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="M12" s="0" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="N12" s="0" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="0" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="E13" s="0" t="s">
         <v>18</v>
@@ -784,22 +820,22 @@
         <v>19</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="K13" s="0" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="L13" s="0" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="M13" s="0" t="s">
         <v>26</v>
@@ -810,13 +846,13 @@
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="0" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>17</v>
@@ -825,19 +861,19 @@
         <v>18</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="K14" s="0" t="s">
         <v>24</v>
@@ -854,16 +890,16 @@
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="0" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="E15" s="0" t="s">
         <v>18</v>
@@ -878,22 +914,66 @@
         <v>21</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="K15" s="0" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="L15" s="0" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="M15" s="0" t="s">
-        <v>26</v>
+        <v>62</v>
       </c>
       <c r="N15" s="0" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="G16" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H16" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="I16" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="J16" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="K16" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="L16" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="M16" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="N16" s="0" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>